<commit_message>
Update laboratory scorecard (minor change)
</commit_message>
<xml_diff>
--- a/docs/Scorecard_laboratory.xlsx
+++ b/docs/Scorecard_laboratory.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="12375" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="10" r:id="rId1"/>
@@ -1291,18 +1291,6 @@
     <t>Construction type: PNNL's CBECS Study</t>
   </si>
   <si>
-    <t>Requirements in codes or standards
-Nonresidential; Walls, Above-Grade, Steel-Framed
-Wall U-factor (Btu/h*ft2*°F): 
-ASHRAE 90.1 2004: 0.084, 2007: 0.064, 2010: 0.064, 2013: 0.055, and 2016: 0.055</t>
-  </si>
-  <si>
-    <t>Requirements in codes or standards
-Nonresidential; Roofs, Insulation entirely above deck
-Roof U-factor (Btu/h*ft2*°F): 
-ASHRAE 90.1 2004: 0.063, 2007: 0.048, 2010:, 0.048, 2013: 0.032, and 2016: 0.032</t>
-  </si>
-  <si>
     <t>PNNL-18898. Infiltration Modeling Guidelines for Commercial Building Energy Analysis.
 Modeled peak infiltration rate may be different for different codes or standards because of their continuous air barrier requirements.</t>
   </si>
@@ -1710,6 +1698,14 @@
   <si>
     <t>Requirements in codes or standards
 Nonresidential; vertical glazing</t>
+  </si>
+  <si>
+    <t>Requirements in codes or standards
+Nonresidential; Roofs, Insulation entirely above deck</t>
+  </si>
+  <si>
+    <t>Requirements in codes or standards
+Nonresidential; Walls, Above-Grade, Steel-Framed</t>
   </si>
 </sst>
 </file>
@@ -3400,12 +3396,393 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3436,36 +3813,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3526,367 +3879,10 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="52" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4584,7 +4580,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4633,7 +4629,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4995,8 +4991,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView zoomScale="181" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5072,8 +5068,8 @@
   </sheetPr>
   <dimension ref="A1:Q149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:F41"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -5084,7 +5080,7 @@
     <col min="4" max="4" width="49.7109375" style="68" customWidth="1"/>
     <col min="5" max="5" width="28" style="68" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" style="68" customWidth="1"/>
-    <col min="7" max="7" width="44.42578125" style="55" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" style="55" customWidth="1"/>
     <col min="8" max="13" width="7.7109375" style="14"/>
     <col min="14" max="14" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="7.7109375" style="14"/>
@@ -5116,44 +5112,44 @@
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="262"/>
-      <c r="B3" s="265" t="s">
+      <c r="A3" s="381"/>
+      <c r="B3" s="384" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="266"/>
-      <c r="D3" s="265" t="s">
+      <c r="C3" s="385"/>
+      <c r="D3" s="384" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="271"/>
-      <c r="F3" s="266"/>
-      <c r="G3" s="234" t="s">
+      <c r="E3" s="390"/>
+      <c r="F3" s="385"/>
+      <c r="G3" s="361" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="263"/>
-      <c r="B4" s="267"/>
-      <c r="C4" s="268"/>
-      <c r="D4" s="267"/>
-      <c r="E4" s="272"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="235"/>
+      <c r="A4" s="382"/>
+      <c r="B4" s="386"/>
+      <c r="C4" s="387"/>
+      <c r="D4" s="386"/>
+      <c r="E4" s="391"/>
+      <c r="F4" s="387"/>
+      <c r="G4" s="362"/>
     </row>
     <row r="5" spans="1:7" s="16" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="264"/>
-      <c r="B5" s="269"/>
-      <c r="C5" s="270"/>
-      <c r="D5" s="269"/>
-      <c r="E5" s="273"/>
-      <c r="F5" s="270"/>
-      <c r="G5" s="236"/>
+      <c r="A5" s="383"/>
+      <c r="B5" s="388"/>
+      <c r="C5" s="389"/>
+      <c r="D5" s="388"/>
+      <c r="E5" s="392"/>
+      <c r="F5" s="389"/>
+      <c r="G5" s="363"/>
     </row>
     <row r="6" spans="1:7" s="15" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="237" t="s">
+      <c r="A6" s="364" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="238"/>
-      <c r="C6" s="238"/>
+      <c r="B6" s="365"/>
+      <c r="C6" s="365"/>
       <c r="D6" s="58"/>
       <c r="E6" s="58"/>
       <c r="F6" s="58"/>
@@ -5161,77 +5157,77 @@
     </row>
     <row r="7" spans="1:7" s="15" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="239" t="s">
+      <c r="B7" s="366" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="240"/>
-      <c r="D7" s="241" t="s">
+      <c r="C7" s="367"/>
+      <c r="D7" s="368" t="s">
         <v>115</v>
       </c>
-      <c r="E7" s="242"/>
-      <c r="F7" s="243"/>
+      <c r="E7" s="369"/>
+      <c r="F7" s="370"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="72"/>
-      <c r="B8" s="249" t="s">
+      <c r="B8" s="372" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="250"/>
-      <c r="D8" s="296" t="s">
+      <c r="C8" s="350"/>
+      <c r="D8" s="240" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="297"/>
-      <c r="F8" s="298"/>
+      <c r="E8" s="241"/>
+      <c r="F8" s="242"/>
       <c r="G8" s="7" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="72"/>
-      <c r="B9" s="244" t="s">
+      <c r="B9" s="232" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="245"/>
-      <c r="D9" s="251" t="s">
+      <c r="C9" s="233"/>
+      <c r="D9" s="299" t="s">
         <v>258</v>
       </c>
-      <c r="E9" s="252"/>
-      <c r="F9" s="253"/>
+      <c r="E9" s="300"/>
+      <c r="F9" s="301"/>
       <c r="G9" s="8"/>
     </row>
     <row r="10" spans="1:7" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="244" t="s">
+      <c r="B10" s="232" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="245"/>
-      <c r="D10" s="254" t="s">
+      <c r="C10" s="233"/>
+      <c r="D10" s="373" t="s">
         <v>172</v>
       </c>
-      <c r="E10" s="255"/>
-      <c r="F10" s="256"/>
+      <c r="E10" s="374"/>
+      <c r="F10" s="375"/>
       <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
-      <c r="B11" s="257" t="s">
+      <c r="B11" s="376" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="258"/>
-      <c r="D11" s="259" t="s">
+      <c r="C11" s="377"/>
+      <c r="D11" s="378" t="s">
         <v>172</v>
       </c>
-      <c r="E11" s="260"/>
-      <c r="F11" s="261"/>
+      <c r="E11" s="379"/>
+      <c r="F11" s="380"/>
       <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" ht="17.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="282" t="s">
+      <c r="A12" s="255" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="283"/>
-      <c r="C12" s="283"/>
+      <c r="B12" s="256"/>
+      <c r="C12" s="256"/>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
       <c r="F12" s="59"/>
@@ -5239,87 +5235,87 @@
     </row>
     <row r="13" spans="1:7" s="16" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
-      <c r="B13" s="299" t="s">
+      <c r="B13" s="340" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="300"/>
-      <c r="D13" s="276" t="s">
+      <c r="C13" s="341"/>
+      <c r="D13" s="344" t="s">
         <v>283</v>
       </c>
-      <c r="E13" s="277"/>
-      <c r="F13" s="278"/>
+      <c r="E13" s="278"/>
+      <c r="F13" s="279"/>
       <c r="G13" s="69" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
-      <c r="B14" s="274" t="s">
+      <c r="B14" s="342" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="275"/>
-      <c r="D14" s="317" t="s">
+      <c r="C14" s="343"/>
+      <c r="D14" s="351" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="318"/>
-      <c r="F14" s="319"/>
+      <c r="E14" s="352"/>
+      <c r="F14" s="353"/>
       <c r="G14" s="71"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="72"/>
-      <c r="B15" s="274" t="s">
+      <c r="B15" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="275"/>
-      <c r="D15" s="320">
+      <c r="C15" s="343"/>
+      <c r="D15" s="354">
         <v>1.33</v>
       </c>
-      <c r="E15" s="321"/>
-      <c r="F15" s="322"/>
+      <c r="E15" s="355"/>
+      <c r="F15" s="356"/>
       <c r="G15" s="180"/>
     </row>
     <row r="16" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70"/>
-      <c r="B16" s="274" t="s">
+      <c r="B16" s="342" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="275"/>
-      <c r="D16" s="276">
+      <c r="C16" s="343"/>
+      <c r="D16" s="344">
         <v>3</v>
       </c>
-      <c r="E16" s="277"/>
-      <c r="F16" s="278"/>
+      <c r="E16" s="278"/>
+      <c r="F16" s="279"/>
       <c r="G16" s="180"/>
     </row>
     <row r="17" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70"/>
-      <c r="B17" s="274" t="s">
+      <c r="B17" s="342" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="275"/>
-      <c r="D17" s="279" t="s">
-        <v>370</v>
-      </c>
-      <c r="E17" s="280"/>
-      <c r="F17" s="281"/>
+      <c r="C17" s="343"/>
+      <c r="D17" s="333" t="s">
+        <v>368</v>
+      </c>
+      <c r="E17" s="393"/>
+      <c r="F17" s="394"/>
       <c r="G17" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="N17" s="14"/>
       <c r="Q17" s="160"/>
     </row>
     <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="72"/>
-      <c r="B18" s="313" t="s">
+      <c r="B18" s="349" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="250"/>
-      <c r="D18" s="314" t="s">
+      <c r="C18" s="350"/>
+      <c r="D18" s="306" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="315"/>
-      <c r="F18" s="316"/>
-      <c r="G18" s="232"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="308"/>
+      <c r="G18" s="272"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
@@ -5331,99 +5327,99 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="72"/>
-      <c r="B19" s="274" t="s">
+      <c r="B19" s="342" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="275"/>
-      <c r="D19" s="276" t="s">
+      <c r="C19" s="343"/>
+      <c r="D19" s="344" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="277"/>
-      <c r="F19" s="278"/>
-      <c r="G19" s="233"/>
+      <c r="E19" s="278"/>
+      <c r="F19" s="279"/>
+      <c r="G19" s="274"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="72"/>
-      <c r="B20" s="274" t="s">
+      <c r="B20" s="342" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="275"/>
-      <c r="D20" s="306" t="s">
+      <c r="C20" s="343"/>
+      <c r="D20" s="281" t="s">
         <v>285</v>
       </c>
-      <c r="E20" s="307"/>
-      <c r="F20" s="308"/>
+      <c r="E20" s="282"/>
+      <c r="F20" s="283"/>
       <c r="G20" s="71"/>
     </row>
     <row r="21" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="72"/>
-      <c r="B21" s="309" t="s">
+      <c r="B21" s="345" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="310"/>
-      <c r="D21" s="306" t="s">
-        <v>343</v>
-      </c>
-      <c r="E21" s="307"/>
-      <c r="F21" s="308"/>
-      <c r="G21" s="232"/>
+      <c r="C21" s="346"/>
+      <c r="D21" s="281" t="s">
+        <v>341</v>
+      </c>
+      <c r="E21" s="282"/>
+      <c r="F21" s="283"/>
+      <c r="G21" s="272"/>
     </row>
     <row r="22" spans="1:17" ht="186.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="72"/>
-      <c r="B22" s="311"/>
-      <c r="C22" s="312"/>
+      <c r="B22" s="347"/>
+      <c r="C22" s="348"/>
       <c r="D22" s="227" t="s">
-        <v>344</v>
-      </c>
-      <c r="E22" s="297"/>
-      <c r="F22" s="298"/>
-      <c r="G22" s="233"/>
+        <v>342</v>
+      </c>
+      <c r="E22" s="241"/>
+      <c r="F22" s="242"/>
+      <c r="G22" s="274"/>
     </row>
     <row r="23" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="72"/>
-      <c r="B23" s="323" t="s">
+      <c r="B23" s="357" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="324"/>
-      <c r="D23" s="291">
+      <c r="C23" s="358"/>
+      <c r="D23" s="259">
         <v>15</v>
       </c>
-      <c r="E23" s="292"/>
-      <c r="F23" s="293"/>
+      <c r="E23" s="260"/>
+      <c r="F23" s="261"/>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="244" t="s">
+      <c r="B24" s="232" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="245"/>
-      <c r="D24" s="291">
+      <c r="C24" s="233"/>
+      <c r="D24" s="259">
         <v>10</v>
       </c>
-      <c r="E24" s="292"/>
-      <c r="F24" s="293"/>
+      <c r="E24" s="260"/>
+      <c r="F24" s="261"/>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="301" t="s">
+      <c r="B25" s="262" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="302"/>
-      <c r="D25" s="303" t="s">
+      <c r="C25" s="263"/>
+      <c r="D25" s="264" t="s">
         <v>235</v>
       </c>
-      <c r="E25" s="304"/>
-      <c r="F25" s="305"/>
+      <c r="E25" s="265"/>
+      <c r="F25" s="266"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="287" t="s">
+      <c r="A26" s="302" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="288"/>
-      <c r="C26" s="288"/>
+      <c r="B26" s="303"/>
+      <c r="C26" s="303"/>
       <c r="D26" s="60"/>
       <c r="E26" s="60"/>
       <c r="F26" s="60"/>
@@ -5431,77 +5427,77 @@
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18"/>
-      <c r="B27" s="289" t="s">
+      <c r="B27" s="359" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="290"/>
+      <c r="C27" s="360"/>
       <c r="D27" s="61"/>
       <c r="E27" s="61"/>
       <c r="F27" s="61"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="16" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70"/>
-      <c r="B28" s="244" t="s">
+      <c r="B28" s="232" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="245"/>
-      <c r="D28" s="291" t="s">
+      <c r="C28" s="233"/>
+      <c r="D28" s="259" t="s">
         <v>105</v>
       </c>
-      <c r="E28" s="292"/>
-      <c r="F28" s="293"/>
+      <c r="E28" s="260"/>
+      <c r="F28" s="261"/>
       <c r="G28" s="7" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="76" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" s="76" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="75"/>
-      <c r="B29" s="294" t="s">
+      <c r="B29" s="267" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="295"/>
-      <c r="D29" s="296" t="s">
-        <v>315</v>
-      </c>
-      <c r="E29" s="297"/>
-      <c r="F29" s="298"/>
+      <c r="C29" s="268"/>
+      <c r="D29" s="240" t="s">
+        <v>396</v>
+      </c>
+      <c r="E29" s="241"/>
+      <c r="F29" s="242"/>
       <c r="G29" s="161" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="72"/>
-      <c r="B30" s="244" t="s">
+      <c r="B30" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="245"/>
-      <c r="D30" s="246" t="s">
+      <c r="C30" s="233"/>
+      <c r="D30" s="237" t="s">
         <v>175</v>
       </c>
-      <c r="E30" s="247"/>
-      <c r="F30" s="284"/>
+      <c r="E30" s="238"/>
+      <c r="F30" s="239"/>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="72"/>
-      <c r="B31" s="244" t="s">
+      <c r="B31" s="232" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="245"/>
-      <c r="D31" s="246" t="s">
+      <c r="C31" s="233"/>
+      <c r="D31" s="237" t="s">
         <v>176</v>
       </c>
-      <c r="E31" s="247"/>
-      <c r="F31" s="284"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="239"/>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:17" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="72"/>
-      <c r="B32" s="285" t="s">
+      <c r="B32" s="309" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="286"/>
+      <c r="C32" s="310"/>
       <c r="D32" s="62"/>
       <c r="E32" s="62"/>
       <c r="F32" s="62"/>
@@ -5509,66 +5505,66 @@
     </row>
     <row r="33" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="72"/>
-      <c r="B33" s="244" t="s">
+      <c r="B33" s="232" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="245"/>
-      <c r="D33" s="246" t="s">
+      <c r="C33" s="233"/>
+      <c r="D33" s="237" t="s">
         <v>237</v>
       </c>
-      <c r="E33" s="247"/>
-      <c r="F33" s="284"/>
+      <c r="E33" s="238"/>
+      <c r="F33" s="239"/>
       <c r="G33" s="7" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="16" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" s="16" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70"/>
-      <c r="B34" s="244" t="s">
+      <c r="B34" s="232" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="245"/>
-      <c r="D34" s="296" t="s">
-        <v>316</v>
-      </c>
-      <c r="E34" s="297"/>
-      <c r="F34" s="298"/>
+      <c r="C34" s="233"/>
+      <c r="D34" s="240" t="s">
+        <v>395</v>
+      </c>
+      <c r="E34" s="241"/>
+      <c r="F34" s="242"/>
       <c r="G34" s="161" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="72"/>
-      <c r="B35" s="244" t="s">
+      <c r="B35" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="245"/>
-      <c r="D35" s="246" t="s">
+      <c r="C35" s="233"/>
+      <c r="D35" s="237" t="s">
         <v>177</v>
       </c>
-      <c r="E35" s="247"/>
-      <c r="F35" s="284"/>
+      <c r="E35" s="238"/>
+      <c r="F35" s="239"/>
       <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="72"/>
-      <c r="B36" s="244" t="s">
+      <c r="B36" s="232" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="245"/>
-      <c r="D36" s="246" t="s">
+      <c r="C36" s="233"/>
+      <c r="D36" s="237" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="247"/>
-      <c r="F36" s="284"/>
+      <c r="E36" s="238"/>
+      <c r="F36" s="239"/>
       <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="72"/>
-      <c r="B37" s="285" t="s">
+      <c r="B37" s="309" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="286"/>
+      <c r="C37" s="310"/>
       <c r="D37" s="62"/>
       <c r="E37" s="62"/>
       <c r="F37" s="62"/>
@@ -5576,80 +5572,80 @@
     </row>
     <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="72"/>
-      <c r="B38" s="244" t="s">
+      <c r="B38" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="245"/>
-      <c r="D38" s="246" t="s">
+      <c r="C38" s="233"/>
+      <c r="D38" s="237" t="s">
         <v>173</v>
       </c>
-      <c r="E38" s="247"/>
-      <c r="F38" s="284"/>
+      <c r="E38" s="238"/>
+      <c r="F38" s="239"/>
       <c r="G38" s="162"/>
     </row>
     <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="72"/>
-      <c r="B39" s="244" t="s">
+      <c r="B39" s="232" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="245"/>
-      <c r="D39" s="246" t="s">
+      <c r="C39" s="233"/>
+      <c r="D39" s="237" t="s">
         <v>174</v>
       </c>
-      <c r="E39" s="315"/>
-      <c r="F39" s="316"/>
+      <c r="E39" s="307"/>
+      <c r="F39" s="308"/>
       <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="70"/>
-      <c r="B40" s="244" t="s">
+      <c r="B40" s="232" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="245"/>
-      <c r="D40" s="325" t="s">
-        <v>396</v>
-      </c>
-      <c r="E40" s="326"/>
-      <c r="F40" s="327"/>
-      <c r="G40" s="232" t="s">
+      <c r="C40" s="233"/>
+      <c r="D40" s="334" t="s">
+        <v>394</v>
+      </c>
+      <c r="E40" s="335"/>
+      <c r="F40" s="336"/>
+      <c r="G40" s="272" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="16" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="70"/>
-      <c r="B41" s="244" t="s">
+      <c r="B41" s="232" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="245"/>
-      <c r="D41" s="328"/>
-      <c r="E41" s="329"/>
-      <c r="F41" s="330"/>
-      <c r="G41" s="233"/>
+      <c r="C41" s="233"/>
+      <c r="D41" s="337"/>
+      <c r="E41" s="338"/>
+      <c r="F41" s="339"/>
+      <c r="G41" s="274"/>
     </row>
     <row r="42" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="72"/>
-      <c r="B42" s="244" t="s">
+      <c r="B42" s="232" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="245"/>
-      <c r="D42" s="246" t="s">
+      <c r="C42" s="233"/>
+      <c r="D42" s="237" t="s">
         <v>232</v>
       </c>
-      <c r="E42" s="315"/>
-      <c r="F42" s="316"/>
+      <c r="E42" s="307"/>
+      <c r="F42" s="308"/>
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="72"/>
-      <c r="B43" s="244" t="s">
+      <c r="B43" s="232" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="245"/>
-      <c r="D43" s="279">
-        <v>0</v>
-      </c>
-      <c r="E43" s="307"/>
-      <c r="F43" s="308"/>
+      <c r="C43" s="233"/>
+      <c r="D43" s="333">
+        <v>0</v>
+      </c>
+      <c r="E43" s="282"/>
+      <c r="F43" s="283"/>
       <c r="G43" s="33" t="s">
         <v>239</v>
       </c>
@@ -5667,62 +5663,62 @@
     </row>
     <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="72"/>
-      <c r="B45" s="244" t="s">
+      <c r="B45" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="245"/>
-      <c r="D45" s="336" t="s">
+      <c r="C45" s="233"/>
+      <c r="D45" s="318" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="337"/>
-      <c r="F45" s="338"/>
+      <c r="E45" s="319"/>
+      <c r="F45" s="320"/>
       <c r="G45" s="26"/>
     </row>
     <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="72"/>
-      <c r="B46" s="244" t="s">
+      <c r="B46" s="232" t="s">
         <v>28</v>
       </c>
-      <c r="C46" s="245"/>
-      <c r="D46" s="339" t="s">
+      <c r="C46" s="233"/>
+      <c r="D46" s="321" t="s">
         <v>34</v>
       </c>
-      <c r="E46" s="340"/>
-      <c r="F46" s="341"/>
-      <c r="G46" s="331"/>
+      <c r="E46" s="322"/>
+      <c r="F46" s="323"/>
+      <c r="G46" s="330"/>
     </row>
     <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="72"/>
-      <c r="B47" s="244" t="s">
+      <c r="B47" s="232" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="245"/>
-      <c r="D47" s="342"/>
-      <c r="E47" s="343"/>
-      <c r="F47" s="344"/>
-      <c r="G47" s="332"/>
+      <c r="C47" s="233"/>
+      <c r="D47" s="324"/>
+      <c r="E47" s="325"/>
+      <c r="F47" s="326"/>
+      <c r="G47" s="331"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="72"/>
-      <c r="B48" s="244" t="s">
+      <c r="B48" s="232" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="245"/>
-      <c r="D48" s="342"/>
-      <c r="E48" s="343"/>
-      <c r="F48" s="344"/>
-      <c r="G48" s="332"/>
+      <c r="C48" s="233"/>
+      <c r="D48" s="324"/>
+      <c r="E48" s="325"/>
+      <c r="F48" s="326"/>
+      <c r="G48" s="331"/>
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="72"/>
-      <c r="B49" s="244" t="s">
+      <c r="B49" s="232" t="s">
         <v>31</v>
       </c>
-      <c r="C49" s="245"/>
-      <c r="D49" s="345"/>
-      <c r="E49" s="346"/>
-      <c r="F49" s="347"/>
-      <c r="G49" s="333"/>
+      <c r="C49" s="233"/>
+      <c r="D49" s="327"/>
+      <c r="E49" s="328"/>
+      <c r="F49" s="329"/>
+      <c r="G49" s="332"/>
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="72"/>
@@ -5737,77 +5733,77 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="72"/>
-      <c r="B51" s="334" t="s">
+      <c r="B51" s="316" t="s">
         <v>36</v>
       </c>
-      <c r="C51" s="335"/>
-      <c r="D51" s="246" t="s">
+      <c r="C51" s="317"/>
+      <c r="D51" s="237" t="s">
         <v>179</v>
       </c>
-      <c r="E51" s="315"/>
-      <c r="F51" s="316"/>
+      <c r="E51" s="307"/>
+      <c r="F51" s="308"/>
       <c r="G51" s="215"/>
     </row>
     <row r="52" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="72"/>
-      <c r="B52" s="244" t="s">
+      <c r="B52" s="232" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="245"/>
-      <c r="D52" s="306" t="s">
+      <c r="C52" s="233"/>
+      <c r="D52" s="281" t="s">
         <v>240</v>
       </c>
-      <c r="E52" s="307"/>
-      <c r="F52" s="308"/>
+      <c r="E52" s="282"/>
+      <c r="F52" s="283"/>
       <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7" s="16" customFormat="1" ht="55.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="70"/>
-      <c r="B53" s="244" t="s">
+      <c r="B53" s="232" t="s">
         <v>37</v>
       </c>
-      <c r="C53" s="245"/>
-      <c r="D53" s="246" t="s">
+      <c r="C53" s="233"/>
+      <c r="D53" s="237" t="s">
         <v>236</v>
       </c>
-      <c r="E53" s="315"/>
-      <c r="F53" s="316"/>
+      <c r="E53" s="307"/>
+      <c r="F53" s="308"/>
       <c r="G53" s="180" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="72"/>
-      <c r="B54" s="244" t="s">
+      <c r="B54" s="232" t="s">
         <v>38</v>
       </c>
-      <c r="C54" s="245"/>
-      <c r="D54" s="246" t="s">
+      <c r="C54" s="233"/>
+      <c r="D54" s="237" t="s">
         <v>34</v>
       </c>
-      <c r="E54" s="315"/>
-      <c r="F54" s="316"/>
+      <c r="E54" s="307"/>
+      <c r="F54" s="308"/>
       <c r="G54" s="23"/>
     </row>
     <row r="55" spans="1:7" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="72"/>
-      <c r="B55" s="244" t="s">
+      <c r="B55" s="232" t="s">
         <v>24</v>
       </c>
-      <c r="C55" s="245"/>
-      <c r="D55" s="246" t="s">
+      <c r="C55" s="233"/>
+      <c r="D55" s="237" t="s">
         <v>177</v>
       </c>
-      <c r="E55" s="247"/>
-      <c r="F55" s="284"/>
+      <c r="E55" s="238"/>
+      <c r="F55" s="239"/>
       <c r="G55" s="23"/>
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="72"/>
-      <c r="B56" s="285" t="s">
+      <c r="B56" s="309" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="286"/>
+      <c r="C56" s="310"/>
       <c r="D56" s="62"/>
       <c r="E56" s="62"/>
       <c r="F56" s="62"/>
@@ -5815,49 +5811,49 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="72"/>
-      <c r="B57" s="244" t="s">
+      <c r="B57" s="232" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="245"/>
-      <c r="D57" s="251" t="s">
+      <c r="C57" s="233"/>
+      <c r="D57" s="299" t="s">
         <v>180</v>
       </c>
-      <c r="E57" s="252"/>
-      <c r="F57" s="253"/>
+      <c r="E57" s="300"/>
+      <c r="F57" s="301"/>
       <c r="G57" s="23"/>
     </row>
     <row r="58" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="72"/>
-      <c r="B58" s="244" t="s">
+      <c r="B58" s="232" t="s">
         <v>41</v>
       </c>
-      <c r="C58" s="245"/>
-      <c r="D58" s="251" t="s">
+      <c r="C58" s="233"/>
+      <c r="D58" s="299" t="s">
         <v>181</v>
       </c>
-      <c r="E58" s="252"/>
-      <c r="F58" s="253"/>
+      <c r="E58" s="300"/>
+      <c r="F58" s="301"/>
       <c r="G58" s="23"/>
     </row>
     <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="72"/>
-      <c r="B59" s="348" t="s">
+      <c r="B59" s="304" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="349"/>
-      <c r="D59" s="314" t="s">
+      <c r="C59" s="305"/>
+      <c r="D59" s="306" t="s">
         <v>182</v>
       </c>
-      <c r="E59" s="315"/>
-      <c r="F59" s="316"/>
+      <c r="E59" s="307"/>
+      <c r="F59" s="308"/>
       <c r="G59" s="23"/>
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="72"/>
-      <c r="B60" s="285" t="s">
+      <c r="B60" s="309" t="s">
         <v>43</v>
       </c>
-      <c r="C60" s="286"/>
+      <c r="C60" s="310"/>
       <c r="D60" s="62"/>
       <c r="E60" s="62"/>
       <c r="F60" s="62"/>
@@ -5865,25 +5861,25 @@
     </row>
     <row r="61" spans="1:7" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="27"/>
-      <c r="B61" s="350" t="s">
-        <v>333</v>
-      </c>
-      <c r="C61" s="351"/>
-      <c r="D61" s="352" t="s">
-        <v>334</v>
-      </c>
-      <c r="E61" s="353"/>
-      <c r="F61" s="354"/>
+      <c r="B61" s="311" t="s">
+        <v>331</v>
+      </c>
+      <c r="C61" s="312"/>
+      <c r="D61" s="313" t="s">
+        <v>332</v>
+      </c>
+      <c r="E61" s="314"/>
+      <c r="F61" s="315"/>
       <c r="G61" s="28" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="287" t="s">
+      <c r="A62" s="302" t="s">
         <v>44</v>
       </c>
-      <c r="B62" s="288"/>
-      <c r="C62" s="288"/>
+      <c r="B62" s="303"/>
+      <c r="C62" s="303"/>
       <c r="D62" s="63"/>
       <c r="E62" s="63"/>
       <c r="F62" s="63"/>
@@ -5902,43 +5898,43 @@
     </row>
     <row r="64" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A64" s="70"/>
-      <c r="B64" s="244" t="s">
+      <c r="B64" s="232" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="245"/>
-      <c r="D64" s="291" t="s">
-        <v>335</v>
-      </c>
-      <c r="E64" s="292"/>
-      <c r="F64" s="293"/>
+      <c r="C64" s="233"/>
+      <c r="D64" s="259" t="s">
+        <v>333</v>
+      </c>
+      <c r="E64" s="260"/>
+      <c r="F64" s="261"/>
       <c r="G64" s="220" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="70"/>
-      <c r="B65" s="244" t="s">
+      <c r="B65" s="232" t="s">
         <v>47</v>
       </c>
-      <c r="C65" s="245"/>
-      <c r="D65" s="291" t="s">
-        <v>372</v>
-      </c>
-      <c r="E65" s="292"/>
-      <c r="F65" s="293"/>
+      <c r="C65" s="233"/>
+      <c r="D65" s="259" t="s">
+        <v>370</v>
+      </c>
+      <c r="E65" s="260"/>
+      <c r="F65" s="261"/>
       <c r="G65" s="219"/>
     </row>
     <row r="66" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="70"/>
-      <c r="B66" s="244" t="s">
+      <c r="B66" s="232" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="245"/>
-      <c r="D66" s="306" t="s">
-        <v>373</v>
-      </c>
-      <c r="E66" s="307"/>
-      <c r="F66" s="308"/>
+      <c r="C66" s="233"/>
+      <c r="D66" s="281" t="s">
+        <v>371</v>
+      </c>
+      <c r="E66" s="282"/>
+      <c r="F66" s="283"/>
       <c r="G66" s="79"/>
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5954,28 +5950,28 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="70"/>
-      <c r="B68" s="244" t="s">
+      <c r="B68" s="232" t="s">
         <v>50</v>
       </c>
-      <c r="C68" s="245"/>
-      <c r="D68" s="251" t="s">
+      <c r="C68" s="233"/>
+      <c r="D68" s="299" t="s">
         <v>183</v>
       </c>
-      <c r="E68" s="252"/>
-      <c r="F68" s="253"/>
+      <c r="E68" s="300"/>
+      <c r="F68" s="301"/>
       <c r="G68" s="23"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="70"/>
-      <c r="B69" s="244" t="s">
+      <c r="B69" s="232" t="s">
         <v>51</v>
       </c>
-      <c r="C69" s="245"/>
-      <c r="D69" s="355" t="s">
+      <c r="C69" s="233"/>
+      <c r="D69" s="234" t="s">
         <v>183</v>
       </c>
-      <c r="E69" s="356"/>
-      <c r="F69" s="357"/>
+      <c r="E69" s="235"/>
+      <c r="F69" s="236"/>
       <c r="G69" s="23"/>
     </row>
     <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5991,31 +5987,31 @@
     </row>
     <row r="71" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="70"/>
-      <c r="B71" s="244" t="s">
+      <c r="B71" s="232" t="s">
         <v>50</v>
       </c>
-      <c r="C71" s="245"/>
-      <c r="D71" s="306" t="s">
-        <v>375</v>
-      </c>
-      <c r="E71" s="307"/>
-      <c r="F71" s="308"/>
-      <c r="G71" s="232" t="s">
+      <c r="C71" s="233"/>
+      <c r="D71" s="281" t="s">
+        <v>373</v>
+      </c>
+      <c r="E71" s="282"/>
+      <c r="F71" s="283"/>
+      <c r="G71" s="272" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="70"/>
-      <c r="B72" s="244" t="s">
+      <c r="B72" s="232" t="s">
         <v>51</v>
       </c>
-      <c r="C72" s="245"/>
-      <c r="D72" s="306" t="s">
+      <c r="C72" s="233"/>
+      <c r="D72" s="281" t="s">
         <v>185</v>
       </c>
-      <c r="E72" s="307"/>
-      <c r="F72" s="308"/>
-      <c r="G72" s="233"/>
+      <c r="E72" s="282"/>
+      <c r="F72" s="283"/>
+      <c r="G72" s="274"/>
     </row>
     <row r="73" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="70"/>
@@ -6030,144 +6026,144 @@
     </row>
     <row r="74" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="70"/>
-      <c r="B74" s="244" t="s">
+      <c r="B74" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="C74" s="245"/>
-      <c r="D74" s="251" t="s">
-        <v>386</v>
-      </c>
-      <c r="E74" s="252"/>
-      <c r="F74" s="253"/>
+      <c r="C74" s="233"/>
+      <c r="D74" s="299" t="s">
+        <v>384</v>
+      </c>
+      <c r="E74" s="300"/>
+      <c r="F74" s="301"/>
       <c r="G74" s="230" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A75" s="70"/>
-      <c r="B75" s="244" t="s">
+      <c r="B75" s="232" t="s">
         <v>55</v>
       </c>
-      <c r="C75" s="245"/>
-      <c r="D75" s="355" t="s">
-        <v>385</v>
-      </c>
-      <c r="E75" s="356"/>
-      <c r="F75" s="357"/>
+      <c r="C75" s="233"/>
+      <c r="D75" s="234" t="s">
+        <v>383</v>
+      </c>
+      <c r="E75" s="235"/>
+      <c r="F75" s="236"/>
       <c r="G75" s="230" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A76" s="70"/>
-      <c r="B76" s="244" t="s">
+      <c r="B76" s="232" t="s">
         <v>56</v>
       </c>
-      <c r="C76" s="245"/>
-      <c r="D76" s="355" t="s">
-        <v>395</v>
-      </c>
-      <c r="E76" s="356"/>
-      <c r="F76" s="356"/>
+      <c r="C76" s="233"/>
+      <c r="D76" s="234" t="s">
+        <v>393</v>
+      </c>
+      <c r="E76" s="235"/>
+      <c r="F76" s="235"/>
       <c r="G76" s="213" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="74"/>
-      <c r="B77" s="244" t="s">
+      <c r="B77" s="232" t="s">
         <v>104</v>
       </c>
-      <c r="C77" s="245"/>
-      <c r="D77" s="246" t="s">
+      <c r="C77" s="233"/>
+      <c r="D77" s="237" t="s">
         <v>34</v>
       </c>
-      <c r="E77" s="247"/>
-      <c r="F77" s="248"/>
+      <c r="E77" s="238"/>
+      <c r="F77" s="371"/>
       <c r="G77" s="200" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="70"/>
-      <c r="B78" s="244" t="s">
+      <c r="B78" s="232" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="245"/>
-      <c r="D78" s="306" t="s">
+      <c r="C78" s="233"/>
+      <c r="D78" s="281" t="s">
         <v>34</v>
       </c>
-      <c r="E78" s="307"/>
-      <c r="F78" s="308"/>
+      <c r="E78" s="282"/>
+      <c r="F78" s="283"/>
       <c r="G78" s="169"/>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="70"/>
-      <c r="B79" s="244" t="s">
+      <c r="B79" s="232" t="s">
         <v>58</v>
       </c>
-      <c r="C79" s="245"/>
-      <c r="D79" s="246" t="s">
+      <c r="C79" s="233"/>
+      <c r="D79" s="237" t="s">
         <v>186</v>
       </c>
-      <c r="E79" s="247"/>
-      <c r="F79" s="284"/>
+      <c r="E79" s="238"/>
+      <c r="F79" s="239"/>
       <c r="G79" s="33"/>
     </row>
     <row r="80" spans="1:7" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="70"/>
-      <c r="B80" s="244" t="s">
+      <c r="B80" s="232" t="s">
         <v>59</v>
       </c>
-      <c r="C80" s="245"/>
-      <c r="D80" s="296" t="s">
+      <c r="C80" s="233"/>
+      <c r="D80" s="240" t="s">
         <v>184</v>
       </c>
-      <c r="E80" s="297"/>
-      <c r="F80" s="298"/>
+      <c r="E80" s="241"/>
+      <c r="F80" s="242"/>
       <c r="G80" s="161" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="81" spans="1:7" s="16" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A81" s="70"/>
-      <c r="B81" s="244" t="s">
+      <c r="B81" s="232" t="s">
         <v>60</v>
       </c>
-      <c r="C81" s="245"/>
-      <c r="D81" s="360" t="s">
-        <v>381</v>
-      </c>
-      <c r="E81" s="361"/>
-      <c r="F81" s="362"/>
+      <c r="C81" s="233"/>
+      <c r="D81" s="296" t="s">
+        <v>379</v>
+      </c>
+      <c r="E81" s="297"/>
+      <c r="F81" s="298"/>
       <c r="G81" s="231" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="70"/>
-      <c r="B82" s="244" t="s">
+      <c r="B82" s="232" t="s">
         <v>61</v>
       </c>
-      <c r="C82" s="245"/>
-      <c r="D82" s="291" t="s">
-        <v>0</v>
-      </c>
-      <c r="E82" s="292"/>
-      <c r="F82" s="293"/>
+      <c r="C82" s="233"/>
+      <c r="D82" s="259" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="260"/>
+      <c r="F82" s="261"/>
       <c r="G82" s="33"/>
     </row>
-    <row r="83" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" s="16" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="70"/>
-      <c r="B83" s="244" t="s">
+      <c r="B83" s="232" t="s">
         <v>62</v>
       </c>
-      <c r="C83" s="245"/>
-      <c r="D83" s="291" t="s">
-        <v>378</v>
-      </c>
-      <c r="E83" s="292"/>
-      <c r="F83" s="293"/>
+      <c r="C83" s="233"/>
+      <c r="D83" s="259" t="s">
+        <v>376</v>
+      </c>
+      <c r="E83" s="260"/>
+      <c r="F83" s="261"/>
       <c r="G83" s="26"/>
     </row>
     <row r="84" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6183,44 +6179,44 @@
     </row>
     <row r="85" spans="1:7" s="16" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="70"/>
-      <c r="B85" s="358" t="s">
+      <c r="B85" s="257" t="s">
         <v>64</v>
       </c>
-      <c r="C85" s="359"/>
-      <c r="D85" s="360" t="s">
+      <c r="C85" s="258"/>
+      <c r="D85" s="296" t="s">
         <v>65</v>
       </c>
-      <c r="E85" s="361"/>
-      <c r="F85" s="362"/>
+      <c r="E85" s="297"/>
+      <c r="F85" s="298"/>
       <c r="G85" s="26"/>
     </row>
     <row r="86" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="70"/>
-      <c r="B86" s="363" t="s">
+      <c r="B86" s="284" t="s">
         <v>66</v>
       </c>
-      <c r="C86" s="364"/>
-      <c r="D86" s="365" t="s">
+      <c r="C86" s="285"/>
+      <c r="D86" s="286" t="s">
         <v>231</v>
       </c>
-      <c r="E86" s="366"/>
-      <c r="F86" s="367"/>
-      <c r="G86" s="232" t="s">
+      <c r="E86" s="287"/>
+      <c r="F86" s="288"/>
+      <c r="G86" s="272" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="87" spans="1:7" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="70"/>
-      <c r="B87" s="363" t="s">
+      <c r="B87" s="284" t="s">
         <v>67</v>
       </c>
-      <c r="C87" s="364"/>
-      <c r="D87" s="291" t="s">
+      <c r="C87" s="285"/>
+      <c r="D87" s="259" t="s">
         <v>68</v>
       </c>
-      <c r="E87" s="292"/>
-      <c r="F87" s="293"/>
-      <c r="G87" s="233"/>
+      <c r="E87" s="260"/>
+      <c r="F87" s="261"/>
+      <c r="G87" s="274"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="173"/>
@@ -6235,59 +6231,59 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="173"/>
-      <c r="B89" s="371" t="s">
+      <c r="B89" s="292" t="s">
         <v>64</v>
       </c>
-      <c r="C89" s="372"/>
-      <c r="D89" s="246" t="s">
-        <v>379</v>
-      </c>
-      <c r="E89" s="247"/>
-      <c r="F89" s="284"/>
+      <c r="C89" s="293"/>
+      <c r="D89" s="237" t="s">
+        <v>377</v>
+      </c>
+      <c r="E89" s="238"/>
+      <c r="F89" s="239"/>
       <c r="G89" s="33"/>
     </row>
-    <row r="90" spans="1:7" s="16" customFormat="1" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A90" s="179"/>
-      <c r="B90" s="244" t="s">
+      <c r="B90" s="232" t="s">
         <v>291</v>
       </c>
-      <c r="C90" s="245"/>
-      <c r="D90" s="360" t="s">
-        <v>383</v>
-      </c>
-      <c r="E90" s="361"/>
-      <c r="F90" s="362"/>
+      <c r="C90" s="233"/>
+      <c r="D90" s="296" t="s">
+        <v>381</v>
+      </c>
+      <c r="E90" s="297"/>
+      <c r="F90" s="298"/>
       <c r="G90" s="201" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="173"/>
-      <c r="B91" s="373" t="s">
+      <c r="B91" s="294" t="s">
         <v>287</v>
       </c>
-      <c r="C91" s="374"/>
-      <c r="D91" s="365" t="s">
+      <c r="C91" s="295"/>
+      <c r="D91" s="286" t="s">
         <v>231</v>
       </c>
-      <c r="E91" s="366"/>
-      <c r="F91" s="367"/>
-      <c r="G91" s="232" t="s">
+      <c r="E91" s="287"/>
+      <c r="F91" s="288"/>
+      <c r="G91" s="272" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="173"/>
-      <c r="B92" s="373" t="s">
+      <c r="B92" s="294" t="s">
         <v>288</v>
       </c>
-      <c r="C92" s="374"/>
-      <c r="D92" s="291" t="s">
+      <c r="C92" s="295"/>
+      <c r="D92" s="259" t="s">
         <v>68</v>
       </c>
-      <c r="E92" s="292"/>
-      <c r="F92" s="293"/>
-      <c r="G92" s="233"/>
+      <c r="E92" s="260"/>
+      <c r="F92" s="261"/>
+      <c r="G92" s="274"/>
     </row>
     <row r="93" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="70"/>
@@ -6302,45 +6298,45 @@
     </row>
     <row r="94" spans="1:7" s="16" customFormat="1" ht="50.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="70"/>
-      <c r="B94" s="358" t="s">
+      <c r="B94" s="257" t="s">
         <v>70</v>
       </c>
-      <c r="C94" s="359"/>
-      <c r="D94" s="368" t="s">
-        <v>382</v>
-      </c>
-      <c r="E94" s="369"/>
-      <c r="F94" s="370"/>
+      <c r="C94" s="258"/>
+      <c r="D94" s="289" t="s">
+        <v>380</v>
+      </c>
+      <c r="E94" s="290"/>
+      <c r="F94" s="291"/>
       <c r="G94" s="33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="70"/>
-      <c r="B95" s="244" t="s">
+      <c r="B95" s="232" t="s">
         <v>71</v>
       </c>
-      <c r="C95" s="245"/>
-      <c r="D95" s="355" t="s">
-        <v>318</v>
-      </c>
-      <c r="E95" s="356"/>
-      <c r="F95" s="357"/>
+      <c r="C95" s="233"/>
+      <c r="D95" s="234" t="s">
+        <v>316</v>
+      </c>
+      <c r="E95" s="235"/>
+      <c r="F95" s="236"/>
       <c r="G95" s="33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="70"/>
-      <c r="B96" s="244" t="s">
+      <c r="B96" s="232" t="s">
         <v>72</v>
       </c>
-      <c r="C96" s="245"/>
-      <c r="D96" s="306" t="s">
+      <c r="C96" s="233"/>
+      <c r="D96" s="281" t="s">
         <v>187</v>
       </c>
-      <c r="E96" s="307"/>
-      <c r="F96" s="308"/>
+      <c r="E96" s="282"/>
+      <c r="F96" s="283"/>
       <c r="G96" s="33"/>
     </row>
     <row r="97" spans="1:7" s="16" customFormat="1" ht="38.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6356,28 +6352,28 @@
     </row>
     <row r="98" spans="1:7" s="16" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="70"/>
-      <c r="B98" s="358" t="s">
+      <c r="B98" s="257" t="s">
         <v>74</v>
       </c>
-      <c r="C98" s="359"/>
-      <c r="D98" s="306" t="s">
+      <c r="C98" s="258"/>
+      <c r="D98" s="281" t="s">
         <v>34</v>
       </c>
-      <c r="E98" s="307"/>
-      <c r="F98" s="308"/>
+      <c r="E98" s="282"/>
+      <c r="F98" s="283"/>
       <c r="G98" s="33"/>
     </row>
     <row r="99" spans="1:7" s="16" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="70"/>
-      <c r="B99" s="358" t="s">
+      <c r="B99" s="257" t="s">
         <v>75</v>
       </c>
-      <c r="C99" s="359"/>
-      <c r="D99" s="306" t="s">
+      <c r="C99" s="258"/>
+      <c r="D99" s="281" t="s">
         <v>34</v>
       </c>
-      <c r="E99" s="307"/>
-      <c r="F99" s="308"/>
+      <c r="E99" s="282"/>
+      <c r="F99" s="283"/>
       <c r="G99" s="26"/>
     </row>
     <row r="100" spans="1:7" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -6393,109 +6389,109 @@
     </row>
     <row r="101" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="70"/>
-      <c r="B101" s="244" t="s">
+      <c r="B101" s="232" t="s">
         <v>77</v>
       </c>
-      <c r="C101" s="245"/>
-      <c r="D101" s="355" t="s">
+      <c r="C101" s="233"/>
+      <c r="D101" s="234" t="s">
         <v>188</v>
       </c>
-      <c r="E101" s="356"/>
-      <c r="F101" s="357"/>
+      <c r="E101" s="235"/>
+      <c r="F101" s="236"/>
       <c r="G101" s="218"/>
     </row>
     <row r="102" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="70"/>
-      <c r="B102" s="244" t="s">
+      <c r="B102" s="232" t="s">
         <v>78</v>
       </c>
-      <c r="C102" s="245"/>
-      <c r="D102" s="355" t="s">
+      <c r="C102" s="233"/>
+      <c r="D102" s="234" t="s">
         <v>189</v>
       </c>
-      <c r="E102" s="356"/>
-      <c r="F102" s="357"/>
+      <c r="E102" s="235"/>
+      <c r="F102" s="236"/>
       <c r="G102" s="218"/>
     </row>
     <row r="103" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="70"/>
-      <c r="B103" s="244" t="s">
+      <c r="B103" s="232" t="s">
         <v>79</v>
       </c>
-      <c r="C103" s="245"/>
-      <c r="D103" s="375" t="s">
+      <c r="C103" s="233"/>
+      <c r="D103" s="280" t="s">
         <v>190</v>
       </c>
-      <c r="E103" s="356"/>
-      <c r="F103" s="357"/>
+      <c r="E103" s="235"/>
+      <c r="F103" s="236"/>
       <c r="G103" s="33" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="104" spans="1:7" s="16" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="70"/>
-      <c r="B104" s="294" t="s">
+      <c r="B104" s="267" t="s">
         <v>80</v>
       </c>
-      <c r="C104" s="295"/>
-      <c r="D104" s="306">
+      <c r="C104" s="268"/>
+      <c r="D104" s="281">
         <v>300</v>
       </c>
-      <c r="E104" s="307"/>
-      <c r="F104" s="308"/>
+      <c r="E104" s="282"/>
+      <c r="F104" s="283"/>
       <c r="G104" s="222" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="105" spans="1:7" s="16" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="39"/>
-      <c r="B105" s="244" t="s">
+      <c r="B105" s="232" t="s">
         <v>81</v>
       </c>
-      <c r="C105" s="245"/>
-      <c r="D105" s="355" t="s">
+      <c r="C105" s="233"/>
+      <c r="D105" s="234" t="s">
         <v>191</v>
       </c>
-      <c r="E105" s="356"/>
-      <c r="F105" s="357"/>
+      <c r="E105" s="235"/>
+      <c r="F105" s="236"/>
       <c r="G105" s="221" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="106" spans="1:7" s="16" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="39"/>
-      <c r="B106" s="244" t="s">
+      <c r="B106" s="232" t="s">
+        <v>322</v>
+      </c>
+      <c r="C106" s="233"/>
+      <c r="D106" s="234" t="s">
+        <v>323</v>
+      </c>
+      <c r="E106" s="235"/>
+      <c r="F106" s="236"/>
+      <c r="G106" s="205" t="s">
         <v>324</v>
-      </c>
-      <c r="C106" s="245"/>
-      <c r="D106" s="355" t="s">
-        <v>325</v>
-      </c>
-      <c r="E106" s="356"/>
-      <c r="F106" s="357"/>
-      <c r="G106" s="205" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="107" spans="1:7" s="16" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="39"/>
-      <c r="B107" s="301" t="s">
+      <c r="B107" s="262" t="s">
         <v>82</v>
       </c>
-      <c r="C107" s="302"/>
-      <c r="D107" s="303" t="s">
+      <c r="C107" s="263"/>
+      <c r="D107" s="264" t="s">
         <v>192</v>
       </c>
-      <c r="E107" s="304"/>
-      <c r="F107" s="305"/>
+      <c r="E107" s="265"/>
+      <c r="F107" s="266"/>
       <c r="G107" s="28"/>
     </row>
     <row r="108" spans="1:7" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="282" t="s">
+      <c r="A108" s="255" t="s">
         <v>83</v>
       </c>
-      <c r="B108" s="283"/>
-      <c r="C108" s="283"/>
+      <c r="B108" s="256"/>
+      <c r="C108" s="256"/>
       <c r="D108" s="59"/>
       <c r="E108" s="59"/>
       <c r="F108" s="59"/>
@@ -6514,60 +6510,60 @@
     </row>
     <row r="110" spans="1:7" s="16" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="45"/>
-      <c r="B110" s="294" t="s">
+      <c r="B110" s="267" t="s">
         <v>84</v>
       </c>
-      <c r="C110" s="295"/>
-      <c r="D110" s="376" t="s">
-        <v>321</v>
-      </c>
-      <c r="E110" s="377"/>
-      <c r="F110" s="378"/>
+      <c r="C110" s="268"/>
+      <c r="D110" s="269" t="s">
+        <v>319</v>
+      </c>
+      <c r="E110" s="270"/>
+      <c r="F110" s="271"/>
       <c r="G110" s="215" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="111" spans="1:7" s="16" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="45"/>
-      <c r="B111" s="244" t="s">
+      <c r="B111" s="232" t="s">
         <v>85</v>
       </c>
-      <c r="C111" s="245"/>
-      <c r="D111" s="291" t="s">
+      <c r="C111" s="233"/>
+      <c r="D111" s="259" t="s">
         <v>65</v>
       </c>
-      <c r="E111" s="292"/>
-      <c r="F111" s="293"/>
+      <c r="E111" s="260"/>
+      <c r="F111" s="261"/>
       <c r="G111" s="215" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="112" spans="1:7" s="16" customFormat="1" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="45"/>
-      <c r="B112" s="244" t="s">
+      <c r="B112" s="232" t="s">
         <v>86</v>
       </c>
-      <c r="C112" s="245"/>
-      <c r="D112" s="355" t="s">
+      <c r="C112" s="233"/>
+      <c r="D112" s="234" t="s">
         <v>190</v>
       </c>
-      <c r="E112" s="356"/>
-      <c r="F112" s="357"/>
+      <c r="E112" s="235"/>
+      <c r="F112" s="236"/>
       <c r="G112" s="33" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="46"/>
-      <c r="B113" s="244" t="s">
+      <c r="B113" s="232" t="s">
         <v>87</v>
       </c>
-      <c r="C113" s="245"/>
-      <c r="D113" s="355" t="s">
+      <c r="C113" s="233"/>
+      <c r="D113" s="234" t="s">
         <v>190</v>
       </c>
-      <c r="E113" s="356"/>
-      <c r="F113" s="357"/>
+      <c r="E113" s="235"/>
+      <c r="F113" s="236"/>
       <c r="G113" s="33" t="s">
         <v>230</v>
       </c>
@@ -6585,32 +6581,32 @@
     </row>
     <row r="115" spans="1:7" s="16" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A115" s="45"/>
-      <c r="B115" s="358" t="s">
+      <c r="B115" s="257" t="s">
         <v>84</v>
       </c>
-      <c r="C115" s="359"/>
-      <c r="D115" s="291" t="s">
-        <v>384</v>
-      </c>
-      <c r="E115" s="292"/>
-      <c r="F115" s="293"/>
+      <c r="C115" s="258"/>
+      <c r="D115" s="259" t="s">
+        <v>382</v>
+      </c>
+      <c r="E115" s="260"/>
+      <c r="F115" s="261"/>
       <c r="G115" s="215" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="116" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="46"/>
-      <c r="B116" s="358" t="s">
+      <c r="B116" s="257" t="s">
         <v>85</v>
       </c>
-      <c r="C116" s="359"/>
-      <c r="D116" s="291" t="s">
+      <c r="C116" s="258"/>
+      <c r="D116" s="259" t="s">
         <v>65</v>
       </c>
-      <c r="E116" s="292"/>
-      <c r="F116" s="293"/>
+      <c r="E116" s="260"/>
+      <c r="F116" s="261"/>
       <c r="G116" s="216" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -6626,40 +6622,40 @@
     </row>
     <row r="118" spans="1:7" s="16" customFormat="1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A118" s="45"/>
-      <c r="B118" s="244" t="s">
+      <c r="B118" s="232" t="s">
         <v>90</v>
       </c>
-      <c r="C118" s="245"/>
-      <c r="D118" s="291" t="s">
-        <v>364</v>
-      </c>
-      <c r="E118" s="277"/>
-      <c r="F118" s="278"/>
+      <c r="C118" s="233"/>
+      <c r="D118" s="259" t="s">
+        <v>362</v>
+      </c>
+      <c r="E118" s="278"/>
+      <c r="F118" s="279"/>
       <c r="G118" s="215" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="50"/>
-      <c r="B119" s="301" t="s">
+      <c r="B119" s="262" t="s">
         <v>85</v>
       </c>
-      <c r="C119" s="302"/>
-      <c r="D119" s="291" t="s">
+      <c r="C119" s="263"/>
+      <c r="D119" s="259" t="s">
         <v>65</v>
       </c>
-      <c r="E119" s="292"/>
-      <c r="F119" s="293"/>
+      <c r="E119" s="260"/>
+      <c r="F119" s="261"/>
       <c r="G119" s="217" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="282" t="s">
+      <c r="A120" s="255" t="s">
         <v>91</v>
       </c>
-      <c r="B120" s="283"/>
-      <c r="C120" s="283"/>
+      <c r="B120" s="256"/>
+      <c r="C120" s="256"/>
       <c r="D120" s="59"/>
       <c r="E120" s="59"/>
       <c r="F120" s="59"/>
@@ -6678,84 +6674,84 @@
     </row>
     <row r="122" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="46"/>
-      <c r="B122" s="380" t="s">
+      <c r="B122" s="244" t="s">
         <v>93</v>
       </c>
-      <c r="C122" s="381"/>
-      <c r="D122" s="296">
+      <c r="C122" s="245"/>
+      <c r="D122" s="240">
         <v>2</v>
       </c>
-      <c r="E122" s="297"/>
-      <c r="F122" s="298"/>
-      <c r="G122" s="232" t="s">
-        <v>342</v>
+      <c r="E122" s="241"/>
+      <c r="F122" s="242"/>
+      <c r="G122" s="272" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="123" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="46"/>
-      <c r="B123" s="380" t="s">
+      <c r="B123" s="244" t="s">
         <v>94</v>
       </c>
-      <c r="C123" s="381"/>
-      <c r="D123" s="296" t="s">
+      <c r="C123" s="245"/>
+      <c r="D123" s="240" t="s">
         <v>220</v>
       </c>
-      <c r="E123" s="297"/>
-      <c r="F123" s="298"/>
-      <c r="G123" s="379"/>
+      <c r="E123" s="241"/>
+      <c r="F123" s="242"/>
+      <c r="G123" s="273"/>
     </row>
     <row r="124" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="46"/>
-      <c r="B124" s="380" t="s">
+      <c r="B124" s="244" t="s">
         <v>95</v>
       </c>
-      <c r="C124" s="381"/>
-      <c r="D124" s="382">
+      <c r="C124" s="245"/>
+      <c r="D124" s="275">
         <v>16055</v>
       </c>
-      <c r="E124" s="383"/>
-      <c r="F124" s="384"/>
-      <c r="G124" s="379"/>
+      <c r="E124" s="276"/>
+      <c r="F124" s="277"/>
+      <c r="G124" s="273"/>
     </row>
     <row r="125" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="46"/>
-      <c r="B125" s="380" t="s">
+      <c r="B125" s="244" t="s">
         <v>96</v>
       </c>
-      <c r="C125" s="381"/>
-      <c r="D125" s="385" t="s">
+      <c r="C125" s="245"/>
+      <c r="D125" s="246" t="s">
         <v>221</v>
       </c>
-      <c r="E125" s="386"/>
-      <c r="F125" s="387"/>
-      <c r="G125" s="233"/>
+      <c r="E125" s="247"/>
+      <c r="F125" s="248"/>
+      <c r="G125" s="274"/>
     </row>
     <row r="126" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="46"/>
-      <c r="B126" s="380" t="s">
+      <c r="B126" s="244" t="s">
         <v>97</v>
       </c>
-      <c r="C126" s="381"/>
-      <c r="D126" s="385">
+      <c r="C126" s="245"/>
+      <c r="D126" s="246">
         <v>161.9</v>
       </c>
-      <c r="E126" s="386"/>
-      <c r="F126" s="387"/>
+      <c r="E126" s="247"/>
+      <c r="F126" s="248"/>
       <c r="G126" s="33" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="46"/>
-      <c r="B127" s="380" t="s">
+      <c r="B127" s="244" t="s">
         <v>98</v>
       </c>
-      <c r="C127" s="381"/>
-      <c r="D127" s="246" t="s">
+      <c r="C127" s="245"/>
+      <c r="D127" s="237" t="s">
         <v>192</v>
       </c>
-      <c r="E127" s="247"/>
-      <c r="F127" s="284"/>
+      <c r="E127" s="238"/>
+      <c r="F127" s="239"/>
       <c r="G127" s="33" t="s">
         <v>257</v>
       </c>
@@ -6773,40 +6769,40 @@
     </row>
     <row r="129" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="53"/>
-      <c r="B129" s="380" t="s">
+      <c r="B129" s="244" t="s">
         <v>100</v>
       </c>
-      <c r="C129" s="389"/>
-      <c r="D129" s="355" t="s">
+      <c r="C129" s="249"/>
+      <c r="D129" s="234" t="s">
         <v>222</v>
       </c>
-      <c r="E129" s="356"/>
-      <c r="F129" s="357"/>
+      <c r="E129" s="235"/>
+      <c r="F129" s="236"/>
       <c r="G129" s="169" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="130" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="50"/>
-      <c r="B130" s="390" t="s">
+      <c r="B130" s="250" t="s">
         <v>85</v>
       </c>
-      <c r="C130" s="391"/>
-      <c r="D130" s="392" t="s">
+      <c r="C130" s="251"/>
+      <c r="D130" s="252" t="s">
         <v>223</v>
       </c>
-      <c r="E130" s="393"/>
-      <c r="F130" s="394"/>
+      <c r="E130" s="253"/>
+      <c r="F130" s="254"/>
       <c r="G130" s="214" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="388" t="s">
+      <c r="A131" s="243" t="s">
         <v>101</v>
       </c>
-      <c r="B131" s="388"/>
-      <c r="C131" s="388"/>
+      <c r="B131" s="243"/>
+      <c r="C131" s="243"/>
       <c r="G131" s="54"/>
     </row>
     <row r="132" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -6824,7 +6820,7 @@
         <v>2</v>
       </c>
       <c r="B133" s="78" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C133" s="77"/>
       <c r="G133" s="54"/>
@@ -6846,7 +6842,7 @@
         <v>4</v>
       </c>
       <c r="B135" s="212" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6854,7 +6850,7 @@
         <v>5</v>
       </c>
       <c r="B136" s="172" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="137" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6862,7 +6858,7 @@
         <v>6</v>
       </c>
       <c r="B137" s="172" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -6870,7 +6866,7 @@
         <v>7</v>
       </c>
       <c r="B138" s="172" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6930,7 +6926,7 @@
         <v>13</v>
       </c>
       <c r="B144" s="172" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
@@ -6938,7 +6934,7 @@
         <v>14</v>
       </c>
       <c r="B145" s="172" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
@@ -6946,7 +6942,7 @@
         <v>15</v>
       </c>
       <c r="B146" s="172" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
@@ -6960,6 +6956,197 @@
     </row>
   </sheetData>
   <mergeCells count="215">
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D3:F5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D40:F41"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="G46:G49"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:F49"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:F68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:F66"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="G91:G92"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:F99"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="G122:G125"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="D123:F123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="D124:F124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="D125:F125"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D111:F111"/>
     <mergeCell ref="B106:C106"/>
     <mergeCell ref="D106:F106"/>
     <mergeCell ref="D127:F127"/>
@@ -6984,197 +7171,6 @@
     <mergeCell ref="B107:C107"/>
     <mergeCell ref="D107:F107"/>
     <mergeCell ref="A108:C108"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="G122:G125"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="D123:F123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="D124:F124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="D125:F125"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:F99"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="G91:G92"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:F66"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:F49"/>
-    <mergeCell ref="G46:G49"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D40:F41"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D3:F5"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:G7 A23 A78:F80 A34:F34 A29:F29 A74:C77 A14:G14 A115:F115 A81:C81 A112:G114 A111:C111 A57:C59 G57:G59 B1:G2 D23:F23 A9:G12 A8:D8 G8 A13:B13 D13:F13 A15:F16 A24:G28 A30:G33 A120:G130 A119:C119 A35:G39 G110:G113 A116:G118 G119 A42:G52 G40 A40:D40 A41:C41 G131:G134 A66:G73 A65:F65 A60:G64 A54:G56 A53:F53 A107:G110 A106 G106 A91:G93 A17:G21 A22:E22 G22 A86:G89 A85:C85 G85 A82:G84 A95:G105 A94:C94 G94">
     <cfRule type="containsText" dxfId="57" priority="87" operator="containsText" text="~??~">
@@ -7521,7 +7517,7 @@
     </row>
     <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="106" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B4" s="107">
         <v>10500</v>
@@ -7570,7 +7566,7 @@
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="106" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B5" s="107">
         <v>3000</v>
@@ -7619,7 +7615,7 @@
     </row>
     <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="106" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B6" s="107">
         <v>1500</v>
@@ -7667,7 +7663,7 @@
     </row>
     <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="106" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B7" s="107">
         <v>10500</v>
@@ -7716,7 +7712,7 @@
     </row>
     <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="106" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B8" s="107">
         <v>3000</v>
@@ -7765,7 +7761,7 @@
     </row>
     <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="106" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B9" s="107">
         <v>1500</v>
@@ -7813,7 +7809,7 @@
     </row>
     <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="106" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B10" s="107">
         <v>10500</v>
@@ -7862,7 +7858,7 @@
     </row>
     <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="106" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B11" s="107">
         <v>3000</v>
@@ -7911,7 +7907,7 @@
     </row>
     <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="106" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B12" s="107">
         <v>1500</v>
@@ -8819,7 +8815,7 @@
     </row>
     <row r="33" spans="1:14" s="225" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="223" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B33" s="223"/>
       <c r="C33" s="223"/>
@@ -8838,7 +8834,7 @@
     <row r="34" spans="1:14" s="225" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="223"/>
       <c r="B34" s="223" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C34" s="223"/>
       <c r="D34" s="224"/>
@@ -8856,7 +8852,7 @@
     <row r="35" spans="1:14" s="225" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="223"/>
       <c r="B35" s="226" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C35" s="223"/>
       <c r="D35" s="224"/>
@@ -8874,7 +8870,7 @@
     <row r="36" spans="1:14" s="225" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="223"/>
       <c r="B36" s="226" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C36" s="223"/>
       <c r="D36" s="224"/>
@@ -8892,7 +8888,7 @@
     <row r="37" spans="1:14" s="225" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="223"/>
       <c r="B37" s="223" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C37" s="223"/>
       <c r="D37" s="224"/>
@@ -9083,7 +9079,7 @@
     </row>
     <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="132" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B5" s="133">
         <v>10500</v>
@@ -9092,7 +9088,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="159" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E5" s="135">
         <f>'Zone Summary'!N4</f>
@@ -9141,7 +9137,7 @@
     </row>
     <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="140" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B6" s="141">
         <v>3000</v>
@@ -9150,7 +9146,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="159" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E6" s="135">
         <f>'Zone Summary'!N5</f>
@@ -9199,7 +9195,7 @@
     </row>
     <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="140" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B7" s="141">
         <v>1500</v>
@@ -9208,46 +9204,46 @@
         <v>1</v>
       </c>
       <c r="D7" s="159" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E7" s="135">
         <f>'Zone Summary'!N6</f>
         <v>0</v>
       </c>
       <c r="F7" s="136" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J7" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N7" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="O7" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="140" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B8" s="141">
         <v>10500</v>
@@ -9256,7 +9252,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="159" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E8" s="135">
         <f>'Zone Summary'!N7</f>
@@ -9305,7 +9301,7 @@
     </row>
     <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="140" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B9" s="141">
         <v>3000</v>
@@ -9314,7 +9310,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="159" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E9" s="135">
         <f>'Zone Summary'!N8</f>
@@ -9363,7 +9359,7 @@
     </row>
     <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="140" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B10" s="141">
         <v>1500</v>
@@ -9372,46 +9368,46 @@
         <v>1</v>
       </c>
       <c r="D10" s="159" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E10" s="135">
         <f>'Zone Summary'!N9</f>
         <v>0</v>
       </c>
       <c r="F10" s="136" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J10" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N10" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="O10" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="140" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B11" s="141">
         <v>10500</v>
@@ -9420,7 +9416,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="159" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E11" s="135">
         <f>'Zone Summary'!N10</f>
@@ -9469,7 +9465,7 @@
     </row>
     <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="140" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B12" s="141">
         <v>3000</v>
@@ -9478,7 +9474,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="159" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E12" s="135">
         <f>'Zone Summary'!N11</f>
@@ -9527,7 +9523,7 @@
     </row>
     <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="140" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B13" s="141">
         <v>1500</v>
@@ -9536,41 +9532,41 @@
         <v>1</v>
       </c>
       <c r="D13" s="159" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E13" s="135">
         <f>'Zone Summary'!N12</f>
         <v>0</v>
       </c>
       <c r="F13" s="136" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J13" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="M13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N13" s="189" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="O13" s="137" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
@@ -10348,12 +10344,12 @@
     </row>
     <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="195" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="152" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="229" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -10622,7 +10618,7 @@
         <v>0.2</v>
       </c>
       <c r="AC4" s="86" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -10981,7 +10977,7 @@
         <v>0.2</v>
       </c>
       <c r="AC9" s="86" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -11340,7 +11336,7 @@
         <v>0.05</v>
       </c>
       <c r="AC14" s="86" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -11615,16 +11611,16 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" s="94" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B19" s="95" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C19" s="164" t="s">
         <v>151</v>
       </c>
       <c r="D19" s="95" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="E19" s="95">
         <v>167</v>
@@ -11653,7 +11649,7 @@
       <c r="AA19" s="95"/>
       <c r="AB19" s="96"/>
       <c r="AC19" s="86" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -13488,7 +13484,7 @@
         <v>0.05</v>
       </c>
       <c r="AC47" s="86" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
@@ -13496,7 +13492,7 @@
       <c r="B48" s="95"/>
       <c r="C48" s="95"/>
       <c r="D48" s="95" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="E48" s="95">
         <v>0.05</v>
@@ -13913,7 +13909,7 @@
     </row>
     <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="94" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B55" s="95" t="s">
         <v>269</v>
@@ -13922,7 +13918,7 @@
         <v>151</v>
       </c>
       <c r="D55" s="95" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E55" s="95">
         <v>0.53</v>
@@ -14002,7 +13998,7 @@
       <c r="B56" s="95"/>
       <c r="C56" s="95"/>
       <c r="D56" s="95" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E56" s="95">
         <v>0.53</v>

</xml_diff>